<commit_message>
addede to test auto push run
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/qs/testdata/CustAddRecord.xlsx
+++ b/src/main/java/com/qa/qs/testdata/CustAddRecord.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sharan6701\Activities\JavaWorkSpace\sharan.automation.qa\src\main\java\com\qa\qs\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C340437-39AF-4191-9E51-46B14B71940F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EB7936-84F0-4D2C-A8EC-A3C6082B375D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6030" yWindow="7635" windowWidth="17295" windowHeight="6870" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CustomerRecord" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="CurrencyCR" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="190">
   <si>
     <t>custKey</t>
   </si>
@@ -318,9 +317,6 @@
     <t>IA</t>
   </si>
   <si>
-    <t>LIFE-SAVING APPLIANCES, SELF-INFLATING</t>
-  </si>
-  <si>
     <t>UN2990</t>
   </si>
   <si>
@@ -414,9 +410,6 @@
     <t>SubClass</t>
   </si>
   <si>
-    <t>ASixty60_1</t>
-  </si>
-  <si>
     <t>Meatal</t>
   </si>
   <si>
@@ -426,12 +419,6 @@
     <t>CC kit</t>
   </si>
   <si>
-    <t>FAK</t>
-  </si>
-  <si>
-    <t>1117.11.1117</t>
-  </si>
-  <si>
     <t>prodCountry</t>
   </si>
   <si>
@@ -459,90 +446,21 @@
     <t>EAR100</t>
   </si>
   <si>
-    <t>SSH_02_01</t>
-  </si>
-  <si>
-    <t>SSH_02_02</t>
-  </si>
-  <si>
-    <t>SSH_02_03</t>
-  </si>
-  <si>
-    <t>SSH2_11</t>
-  </si>
-  <si>
-    <t>SSH2_12</t>
-  </si>
-  <si>
-    <t>SSH2_13</t>
-  </si>
-  <si>
     <t>1119.11.12</t>
   </si>
   <si>
     <t>1119.11.1119</t>
   </si>
   <si>
-    <t>caQQ111</t>
-  </si>
-  <si>
-    <t>caQQ111@epicor.com</t>
-  </si>
-  <si>
-    <t>caQQ211</t>
-  </si>
-  <si>
-    <t>caQQ211@epicor.com</t>
-  </si>
-  <si>
-    <t>caQQ311</t>
-  </si>
-  <si>
-    <t>caQQ311@epicor.com</t>
-  </si>
-  <si>
-    <t>AFifty50_2</t>
-  </si>
-  <si>
-    <t>AFiftyFivf55_2</t>
-  </si>
-  <si>
     <t>ASixty60_2</t>
   </si>
   <si>
-    <t>Sharan_USA-1121</t>
-  </si>
-  <si>
-    <t>Sharan Consulting LTD USA-1121</t>
-  </si>
-  <si>
-    <t>Dhruva  USA-1121</t>
-  </si>
-  <si>
     <t>dhruvaUSA1121@customer.com</t>
   </si>
   <si>
-    <t>Sharan_AUS-1121</t>
-  </si>
-  <si>
-    <t>Sharan Consulting LTD AUS-1121</t>
-  </si>
-  <si>
-    <t>Dhruva  AUS-1121</t>
-  </si>
-  <si>
     <t>dhruvaAUS1121@customer.com</t>
   </si>
   <si>
-    <t>Sharan_CAD-1121</t>
-  </si>
-  <si>
-    <t>Sharan Consulting LTD CAD-1121</t>
-  </si>
-  <si>
-    <t>Dhruva  CAD-1121</t>
-  </si>
-  <si>
     <t>dhruvaCAD1121@customer.com</t>
   </si>
   <si>
@@ -607,6 +525,93 @@
   </si>
   <si>
     <t>Ireland</t>
+  </si>
+  <si>
+    <t>PAINT RELATED MATERIAL1</t>
+  </si>
+  <si>
+    <t>LIFE-SAVING APPLIANCES, SELF-INFLATING1</t>
+  </si>
+  <si>
+    <t>SSH_03_01</t>
+  </si>
+  <si>
+    <t>SSH_03_02</t>
+  </si>
+  <si>
+    <t>SSH_03_03</t>
+  </si>
+  <si>
+    <t>SSH3_11</t>
+  </si>
+  <si>
+    <t>SSH3_12</t>
+  </si>
+  <si>
+    <t>SSH3_13</t>
+  </si>
+  <si>
+    <t>1120.11.12</t>
+  </si>
+  <si>
+    <t>1120.11.1120</t>
+  </si>
+  <si>
+    <t>caRR111</t>
+  </si>
+  <si>
+    <t>caRR111@epicor.com</t>
+  </si>
+  <si>
+    <t>caRR211</t>
+  </si>
+  <si>
+    <t>caRR211@epicor.com</t>
+  </si>
+  <si>
+    <t>caRR311</t>
+  </si>
+  <si>
+    <t>caRR311@epicor.com</t>
+  </si>
+  <si>
+    <t>Fifty50_3</t>
+  </si>
+  <si>
+    <t>FiftyFivf55_3</t>
+  </si>
+  <si>
+    <t>Sixty60_3</t>
+  </si>
+  <si>
+    <t>Sharan_USA-1122</t>
+  </si>
+  <si>
+    <t>Sharan Consulting LTD USA-1122</t>
+  </si>
+  <si>
+    <t>Dhruva  USA-1122</t>
+  </si>
+  <si>
+    <t>Sharan_AUS-1122</t>
+  </si>
+  <si>
+    <t>Sharan Consulting LTD AUS-1122</t>
+  </si>
+  <si>
+    <t>Dhruva  AUS-1122</t>
+  </si>
+  <si>
+    <t>Sharan_CAD-1122</t>
+  </si>
+  <si>
+    <t>Sharan Consulting LTD CAD-1122</t>
+  </si>
+  <si>
+    <t>Dhruva  CAD-1122</t>
+  </si>
+  <si>
+    <t>7777.77.7777</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1089,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,19 +1148,19 @@
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>32</v>
@@ -1181,19 +1186,19 @@
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>161</v>
+        <v>185</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>32</v>
@@ -1219,19 +1224,19 @@
     </row>
     <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>32</v>
@@ -1267,7 +1272,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,24 +1286,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>50</v>
@@ -1315,7 +1320,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>51</v>
@@ -1332,7 +1337,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>52</v>
@@ -1358,7 +1363,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,10 +1398,10 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>41</v>
@@ -1405,7 +1410,7 @@
         <v>41</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>38</v>
@@ -1413,10 +1418,10 @@
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>41</v>
@@ -1425,7 +1430,7 @@
         <v>41</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>39</v>
@@ -1433,10 +1438,10 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>41</v>
@@ -1445,7 +1450,7 @@
         <v>41</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>38</v>
@@ -1473,7 +1478,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1497,7 +1502,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
-        <v>1119.1199999999999</v>
+        <v>1120.1199999999999</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>30</v>
@@ -1508,7 +1513,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>42</v>
@@ -1519,7 +1524,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>29</v>
@@ -1540,7 +1545,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,79 +1584,79 @@
         <v>49</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="B2" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>113</v>
-      </c>
       <c r="G2" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" t="s">
         <v>104</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>115</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>116</v>
       </c>
       <c r="G3" s="21" t="s">
         <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="B4" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>57</v>
@@ -1663,13 +1668,13 @@
         <v>57</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" t="s">
         <v>104</v>
-      </c>
-      <c r="I4" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1683,8 +1688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E07267-5D03-4CBE-BC6C-6350AB7503AA}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,10 +1734,10 @@
         <v>64</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>60</v>
@@ -1755,10 +1760,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" t="s">
         <v>28</v>
@@ -1766,46 +1771,46 @@
       <c r="D2" t="s">
         <v>83</v>
       </c>
-      <c r="E2" t="s">
-        <v>127</v>
+      <c r="E2" s="24" t="s">
+        <v>136</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H2" t="s">
-        <v>128</v>
+      <c r="H2" s="24" t="s">
+        <v>189</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
       </c>
       <c r="J2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2" t="s">
         <v>131</v>
-      </c>
-      <c r="K2" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" t="s">
-        <v>133</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="N2" t="s">
-        <v>134</v>
-      </c>
-      <c r="O2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1813,46 +1818,46 @@
       <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="E3" t="s">
-        <v>123</v>
+      <c r="E3" s="24" t="s">
+        <v>136</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3">
-        <v>1116.1199999999999</v>
+        <v>116</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="I3" t="s">
         <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M3" s="23" t="s">
         <v>57</v>
       </c>
       <c r="N3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -1864,13 +1869,13 @@
         <v>89</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4">
-        <v>1118.1199999999999</v>
+        <v>116</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>134</v>
       </c>
       <c r="I4" t="s">
         <v>89</v>
@@ -1891,7 +1896,7 @@
         <v>89</v>
       </c>
       <c r="O4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1905,7 +1910,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1966,30 +1971,30 @@
         <v>82</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>83</v>
+        <v>161</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>88</v>
@@ -1998,10 +2003,10 @@
         <v>85</v>
       </c>
       <c r="G2" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>102</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>103</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>86</v>
@@ -2019,63 +2024,63 @@
         <v>90</v>
       </c>
       <c r="N2" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="O2" s="18" t="s">
-        <v>105</v>
-      </c>
       <c r="P2" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="G3" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="H3" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>102</v>
-      </c>
       <c r="I3" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>84</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>89</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>104</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2101,79 +2106,79 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="B5" t="b">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="B6" t="b">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2185,7 +2190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17374631-916E-4935-A91B-D5B00F1C7E02}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -2199,16 +2204,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2222,7 +2227,7 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2236,7 +2241,7 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2244,13 +2249,13 @@
         <v>16</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C4">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2258,13 +2263,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2278,7 +2283,7 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>